<commit_message>
added full exp 2 zones prepocessing
</commit_message>
<xml_diff>
--- a/data/Full exp 2/2023_Sept_20_ip_DFP_fullexp2_meta.xlsx
+++ b/data/Full exp 2/2023_Sept_20_ip_DFP_fullexp2_meta.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/karissabarthelson/Documents/2023_iron_chelation_MPSIII/data/Full exp 2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81106065-E183-664F-A708-16F46E736645}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30E94943-F30A-EE41-9C77-95C4837F4372}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38320" yWindow="-11660" windowWidth="25380" windowHeight="20900" xr2:uid="{B5A38CCD-FB06-BD49-96A4-CB022EEABABF}"/>
   </bookViews>
@@ -3089,9 +3089,9 @@
   </sheetPr>
   <dimension ref="A1:P121"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="88" zoomScaleNormal="88" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="O1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="P56" sqref="P56"/>
+    <sheetView tabSelected="1" topLeftCell="A41" zoomScale="88" zoomScaleNormal="88" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="L50" sqref="L50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3109,7 +3109,7 @@
     <col min="13" max="13" width="47.33203125" customWidth="1"/>
     <col min="14" max="14" width="39" customWidth="1"/>
     <col min="15" max="15" width="22.5" customWidth="1"/>
-    <col min="16" max="16" width="45.6640625" customWidth="1"/>
+    <col min="16" max="16" width="14.6640625" customWidth="1"/>
     <col min="17" max="17" width="25.83203125" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>